<commit_message>
config to run all weather years
</commit_message>
<xml_diff>
--- a/data/Analysis/NPV.xlsx
+++ b/data/Analysis/NPV.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9403A9D8-F62C-4270-9C11-CE83F99B5991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C884F1-727A-417D-961A-E32426AF94B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83D55FD4-1814-4229-ACF7-7739455E9410}"/>
+    <workbookView xWindow="-14505" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{83D55FD4-1814-4229-ACF7-7739455E9410}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="npv" sheetId="2" r:id="rId2"/>
+    <sheet name="annuity" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -81,7 +82,145 @@
     <t>npv</t>
   </si>
   <si>
-    <t>rate</t>
+    <t>unprofitable</t>
+  </si>
+  <si>
+    <t>profitable</t>
+  </si>
+  <si>
+    <t>IRR</t>
+  </si>
+  <si>
+    <t>discount rate</t>
+  </si>
+  <si>
+    <t>debt rate</t>
+  </si>
+  <si>
+    <t>equity rate</t>
+  </si>
+  <si>
+    <t>equity percentage</t>
+  </si>
+  <si>
+    <t>debt percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depreciation time </t>
+  </si>
+  <si>
+    <t>construction time</t>
+  </si>
+  <si>
+    <t>downpayment installment</t>
+  </si>
+  <si>
+    <t>wacc</t>
+  </si>
+  <si>
+    <t>annuity</t>
+  </si>
+  <si>
+    <t>downpayment from two years before the start</t>
+  </si>
+  <si>
+    <t>downpayment from 3 years before the start</t>
+  </si>
+  <si>
+    <t>revenues to cover for annuity</t>
+  </si>
+  <si>
+    <t>operating profit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> operating profit - annuity</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>projectValue = discountedOperatingProfit + discountedCapitalCosts;</t>
+  </si>
+  <si>
+    <t>public TreeMap&lt;Integer, Double&gt; calculateSimplePowerPlantInvestmentCashFlow(int depriacationTime, int buildingTime,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        double totalInvestment, double operatingProfit) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    TreeMap&lt;Integer, Double&gt; investmentCashFlow = new TreeMap&lt;Integer, Double&gt;();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double equalTotalDownPaymentInstallement = totalInvestment / buildingTime;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int i = 0; i &lt; buildingTime; i++) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        investmentCashFlow.put(new Integer(i), -equalTotalDownPaymentInstallement);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int i = buildingTime; i &lt; depriacationTime + buildingTime; i++) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    return investmentCashFlow;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        investmentCashFlow.put(new Integer(i), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>operatingProfit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>emlab consider wacc and no equity/financing difference</t>
+  </si>
+  <si>
+    <t>100% equity - &gt; optimization models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old - new : </t>
+  </si>
+  <si>
+    <t>from emlab generation report</t>
+  </si>
+  <si>
+    <t>Rest payment= &gt; but wrong because there are no interest loans</t>
+  </si>
+  <si>
+    <t>with equity and debt 10%</t>
+  </si>
+  <si>
+    <t>with debt 10%</t>
+  </si>
+  <si>
+    <t>considering higher debt rate we are overestimating NPV&gt; overinvestment.  Considering pur way of financing &gt; underinvestment (if debt rate is high)</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>https://fneum.github.io/data-science-for-esm/10-workshop-pypsa-cem.html#from-electricity-market-modelling-to-capacity-expansion-planning</t>
   </si>
 </sst>
 </file>
@@ -91,9 +230,9 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;€&quot;\ #,##0;[Red]&quot;€&quot;\ \-#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;€&quot;\ #,##0.00;[Red]&quot;€&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="171" formatCode="_ &quot;€&quot;\ * #,##0_ ;_ &quot;€&quot;\ * \-#,##0_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ &quot;€&quot;\ * #,##0_ ;_ &quot;€&quot;\ * \-#,##0_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,13 +253,51 @@
       <color rgb="FF808080"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,10 +309,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -146,10 +324,38 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -162,6 +368,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>516059</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>164528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>474944</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>34990</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{824BB176-FFB2-485F-50E3-00DED0469A19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14009809" y="6551163"/>
+          <a:ext cx="6577539" cy="2618058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -463,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAFFDB23-FC54-47A4-8DFC-1B64B62A74F9}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="69" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -1303,415 +1558,1504 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C261F92-D42A-45AF-90F6-72A03AECACA1}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
     <col min="2" max="2" width="17.81640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="2.54296875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" style="8" customWidth="1"/>
+    <col min="5" max="7" width="21.54296875" customWidth="1"/>
+    <col min="8" max="8" width="24.26953125" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7265625" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.36328125" customWidth="1"/>
+    <col min="13" max="13" width="17.453125" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1">
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="7">
+        <f>(-PMT(B5,30,1,0))*B1</f>
+        <v>6505143.5080276579</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="7">
+        <f>(-PMT(0.1,30,1,0))*B1</f>
+        <v>10607924.825263392</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="10">
+        <v>0</v>
+      </c>
+      <c r="O1" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>0.3</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7">
+        <v>12000000</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="8">
+        <f>NPV(N1,$B$18:$B$49)</f>
+        <v>-5000000</v>
+      </c>
+      <c r="O2" s="8">
+        <f>NPV(O1,$B$18:$B$49)</f>
+        <v>-11622471.1896223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="8">
+        <f>NPV(N1,$D$18:$D$49)</f>
+        <v>134845694.75917026</v>
+      </c>
+      <c r="O3" s="8">
+        <f>NPV(O1,$D$18:$D$49)</f>
+        <v>49383766.710915618</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="8">
+        <f>B1*B7/(B3+1)</f>
+        <v>10000000</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="7">
+        <f>E2-E1</f>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7">
+        <f>E2-G1</f>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+    </row>
+    <row r="5" spans="1:15" ht="18.5">
+      <c r="A5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18.5">
+      <c r="A6" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="H6" s="11">
+        <f>J13-E13</f>
+        <v>-5.2664987693848087E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="9">
+        <f>(B8*B5)+( B7*B6)</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" s="13" customFormat="1" ht="45.5" customHeight="1">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="C11" s="9"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9">
+        <f>IRR($B$18:$B$49)</f>
+        <v>-1.7136070233869094E-2</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="11">
+        <f>IRR($D$18:$D$49)</f>
+        <v>0.180238382762685</v>
+      </c>
+      <c r="E13" s="12">
+        <f>IRR($E$17:$E$49)</f>
+        <v>0.15536713917700595</v>
+      </c>
+      <c r="F13" s="9">
+        <f>IRR($F$17:$F$49)</f>
+        <v>2.1263950429343037E-2</v>
+      </c>
+      <c r="G13" s="9">
+        <f>IRR($G$17:$G$49)</f>
+        <v>0.25264368152082506</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="11">
+        <f>IRR($I$19:$I$49)</f>
+        <v>0.1154777580788291</v>
+      </c>
+      <c r="J13" s="11">
+        <f>IRR($J$17:$J$49)</f>
+        <v>0.10270215148315787</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7">
+        <f>NPV(B6,$B$18:$B$49)</f>
+        <v>-13459952.699591607</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7">
+        <f>NPV(B6,$D$18:$D$49)</f>
+        <v>17941019.063875724</v>
+      </c>
+      <c r="E14" s="7">
+        <f>NPV($B$6,$E$17:$E$49)</f>
+        <v>14049242.793537728</v>
+      </c>
+      <c r="F14" s="7">
+        <f>NPV($B$6,$F$17:$F$49)</f>
+        <v>-15009035.609421629</v>
+      </c>
+      <c r="G14" s="7">
+        <f>NPV($B$6,$G$17:$G$49)</f>
+        <v>43596423.627012521</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7">
+        <f>NPV($B$9,$I$19:$I$49)</f>
+        <v>53243296.5934598</v>
+      </c>
+      <c r="J14" s="7">
+        <f>NPV($B$9,$J$17:$J$49)</f>
+        <v>41444838.843094438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="B16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17">
+        <v>-3</v>
+      </c>
+      <c r="E17" s="8">
+        <f>-B4</f>
+        <v>-10000000</v>
+      </c>
+      <c r="F17" s="8">
+        <f>G17</f>
+        <v>-10000000</v>
+      </c>
+      <c r="G17" s="8">
+        <f>E17</f>
+        <v>-10000000</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="J17" s="8">
+        <f>-B1/3</f>
+        <v>-33333333.333333332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18">
         <v>-2</v>
       </c>
-      <c r="B1" s="8">
-        <v>-8664000</v>
-      </c>
-      <c r="C1" s="8">
-        <v>-8664000</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B18" s="8">
+        <f>-B4</f>
+        <v>-10000000</v>
+      </c>
+      <c r="D18" s="8">
+        <f>B18</f>
+        <v>-10000000</v>
+      </c>
+      <c r="E18" s="8">
+        <f>E17</f>
+        <v>-10000000</v>
+      </c>
+      <c r="F18" s="8">
+        <f>G18</f>
+        <v>-10000000</v>
+      </c>
+      <c r="G18" s="8">
+        <f>E18</f>
+        <v>-10000000</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="J18" s="8">
+        <f>J17</f>
+        <v>-33333333.333333332</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19">
+        <v>-1</v>
+      </c>
+      <c r="B19" s="8">
+        <f>-B4</f>
+        <v>-10000000</v>
+      </c>
+      <c r="D19" s="8">
+        <f>B19</f>
+        <v>-10000000</v>
+      </c>
+      <c r="E19" s="8">
+        <f>E18</f>
+        <v>-10000000</v>
+      </c>
+      <c r="F19" s="8">
+        <f>G19</f>
+        <v>-10000000</v>
+      </c>
+      <c r="G19" s="8">
+        <f>E19</f>
+        <v>-10000000</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="8">
+        <f>-B1</f>
+        <v>-100000000</v>
+      </c>
+      <c r="J19" s="8">
+        <f>J18</f>
+        <v>-33333333.333333332</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D20" s="8">
+        <f>-B4 +E4</f>
+        <v>-4505143.5080276579</v>
+      </c>
+      <c r="E20" s="8">
+        <f>E4</f>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F20" s="8">
+        <f>G4</f>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G20" s="8">
+        <f>E2-(B1*B8)/30</f>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="7">
+        <f>E2</f>
+        <v>12000000</v>
+      </c>
+      <c r="J20" s="7">
+        <f>I20</f>
+        <v>12000000</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D21" s="8">
+        <f>E4</f>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E21" s="8">
+        <f>E20</f>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F21" s="8">
+        <f>F20</f>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G21" s="8">
+        <f>G20</f>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="7">
+        <f>I20</f>
+        <v>12000000</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" ref="J21:J49" si="0">I21</f>
+        <v>12000000</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D22" s="8">
+        <f>D21</f>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" ref="E22:E49" si="1">E21</f>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F22" s="8">
+        <f>F21</f>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G22" s="8">
+        <f>G21</f>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="7">
+        <f t="shared" ref="I22:I49" si="2">I21</f>
+        <v>12000000</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="O22" s="9"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D23" s="8">
+        <f t="shared" ref="D23:D49" si="3">D22</f>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E23" s="8">
+        <f>E22</f>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F23" s="8">
+        <f t="shared" ref="F23:F49" si="4">F22</f>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" ref="G23:G49" si="5">G22</f>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D24" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G24" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D25" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F25" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G25" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="7">
+        <f>I24</f>
+        <v>12000000</v>
+      </c>
+      <c r="J25" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D26" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E26" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D27" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F27" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G27" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D28" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E28" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F28" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G28" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H28" s="8"/>
+      <c r="I28" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L28" s="18"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D29" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E29" s="8">
+        <f>E28</f>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F29" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G29" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H29" s="8"/>
+      <c r="I29" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D30" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E30" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G30" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J30" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31">
+        <v>11</v>
+      </c>
+      <c r="B31" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D31" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E31" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F31" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G31" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32">
+        <v>12</v>
+      </c>
+      <c r="B32" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D32" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E32" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G32" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H32" s="8"/>
+      <c r="I32" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J32" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>13</v>
+      </c>
+      <c r="B33" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D33" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E33" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F33" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G33" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H33" s="8"/>
+      <c r="I33" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J33" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
         <v>14</v>
       </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0.05</v>
-      </c>
-      <c r="H1">
+      <c r="B34" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D34" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E34" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F34" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G34" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H34" s="8"/>
+      <c r="I34" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J34" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>15</v>
+      </c>
+      <c r="B35" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D35" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E35" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F35" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G35" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H35" s="8"/>
+      <c r="I35" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J35" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
+        <v>16</v>
+      </c>
+      <c r="B36" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D36" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E36" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F36" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G36" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H36" s="8"/>
+      <c r="I36" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J36" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>17</v>
+      </c>
+      <c r="B37" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D37" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E37" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F37" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G37" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H37" s="8"/>
+      <c r="I37" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J37" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>18</v>
+      </c>
+      <c r="B38" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D38" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E38" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F38" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G38" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H38" s="8"/>
+      <c r="I38" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J38" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39">
+        <v>19</v>
+      </c>
+      <c r="B39" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D39" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E39" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F39" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G39" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J39" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40">
+        <v>20</v>
+      </c>
+      <c r="B40" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D40" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E40" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G40" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H40" s="8"/>
+      <c r="I40" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J40" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41">
+        <v>21</v>
+      </c>
+      <c r="B41" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D41" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E41" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F41" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G41" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H41" s="8"/>
+      <c r="I41" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J41" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42">
+        <v>22</v>
+      </c>
+      <c r="B42" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D42" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E42" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F42" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G42" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H42" s="8"/>
+      <c r="I42" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J42" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43">
+        <v>23</v>
+      </c>
+      <c r="B43" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D43" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E43" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F43" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G43" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H43" s="8"/>
+      <c r="I43" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J43" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44">
+        <v>24</v>
+      </c>
+      <c r="B44" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D44" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E44" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F44" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G44" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H44" s="8"/>
+      <c r="I44" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J44" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45">
+        <v>25</v>
+      </c>
+      <c r="B45" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D45" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E45" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F45" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G45" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H45" s="8"/>
+      <c r="I45" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J45" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46">
+        <v>26</v>
+      </c>
+      <c r="B46" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D46" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E46" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F46" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G46" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H46" s="8"/>
+      <c r="I46" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J46" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47">
+        <v>27</v>
+      </c>
+      <c r="B47" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D47" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E47" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F47" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G47" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H47" s="8"/>
+      <c r="I47" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J47" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48">
+        <v>28</v>
+      </c>
+      <c r="B48" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D48" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E48" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F48" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G48" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H48" s="8"/>
+      <c r="I48" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J48" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49">
+        <v>29</v>
+      </c>
+      <c r="B49" s="8">
+        <v>500000</v>
+      </c>
+      <c r="D49" s="8">
+        <f t="shared" si="3"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="E49" s="8">
+        <f t="shared" si="1"/>
+        <v>5494856.4919723421</v>
+      </c>
+      <c r="F49" s="8">
+        <f t="shared" si="4"/>
+        <v>1392075.1747366078</v>
+      </c>
+      <c r="G49" s="8">
+        <f t="shared" si="5"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H49" s="8"/>
+      <c r="I49" s="7">
+        <f t="shared" si="2"/>
+        <v>12000000</v>
+      </c>
+      <c r="J49" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:J4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C14:J14">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6D81C7-B300-4311-9A03-B873646C37FD}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="20.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="str">
+        <f>npv!A1</f>
+        <v>investment cost</v>
+      </c>
+      <c r="B1">
+        <f>npv!B1</f>
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>-1</v>
-      </c>
-      <c r="B2" s="8">
-        <v>-8664000</v>
-      </c>
-      <c r="C2" s="8">
-        <v>-8664000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="6">
-        <f>NPV(F1,$B$1:$B$30)</f>
-        <v>-17328000</v>
-      </c>
-      <c r="G2" s="6">
-        <f t="shared" ref="G2:H2" si="0">NPV(G1,$B$1:$B$30)</f>
-        <v>-16109931.972789114</v>
-      </c>
-      <c r="H2" s="6">
-        <f>NPV(H1,$B$1:$B$30)</f>
-        <v>-15036694.214876032</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="6">
-        <f>NPV(F1,$C$1:$C$30)</f>
-        <v>10672000</v>
-      </c>
-      <c r="G3" s="6">
-        <f t="shared" ref="G3:H3" si="1">NPV(G1,$C$1:$C$30)</f>
-        <v>-2596891.3767452873</v>
-      </c>
-      <c r="H3" s="6">
-        <f>NPV(H1,$C$1:$C$30)</f>
-        <v>-7345316.9379703617</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" s="8">
-        <v>0</v>
-      </c>
-      <c r="C9" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" s="8">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0</v>
-      </c>
-      <c r="C11" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" s="8">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" s="8">
-        <v>0</v>
-      </c>
-      <c r="C14" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" s="8">
-        <v>0</v>
-      </c>
-      <c r="C15" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" s="8">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
         <v>15</v>
       </c>
-      <c r="B18" s="8">
-        <v>0</v>
-      </c>
-      <c r="C18" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="B19" s="8">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="B20" s="8">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8">
-        <v>0</v>
-      </c>
-      <c r="C21" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>19</v>
-      </c>
-      <c r="B22" s="8">
-        <v>0</v>
-      </c>
-      <c r="C22" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>20</v>
-      </c>
-      <c r="B23" s="8">
-        <v>0</v>
-      </c>
-      <c r="C23" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>21</v>
-      </c>
-      <c r="B24" s="8">
-        <v>0</v>
-      </c>
-      <c r="C24" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25">
-        <v>22</v>
-      </c>
-      <c r="B25" s="8">
-        <v>0</v>
-      </c>
-      <c r="C25" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>23</v>
-      </c>
-      <c r="B26" s="8">
-        <v>0</v>
-      </c>
-      <c r="C26" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>24</v>
-      </c>
-      <c r="B27" s="8">
-        <v>0</v>
-      </c>
-      <c r="C27" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>25</v>
-      </c>
-      <c r="B28" s="8">
-        <v>0</v>
-      </c>
-      <c r="C28" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29">
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="8">
-        <v>0</v>
-      </c>
-      <c r="C29" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30">
-        <v>27</v>
-      </c>
-      <c r="B30" s="8">
-        <v>0</v>
-      </c>
-      <c r="C30" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31">
-        <v>28</v>
-      </c>
-      <c r="B31" s="8">
-        <v>0</v>
-      </c>
-      <c r="C31" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32">
-        <v>29</v>
-      </c>
-      <c r="B32" s="8">
-        <v>0</v>
-      </c>
-      <c r="C32" s="8">
-        <v>1000000</v>
+      <c r="B5">
+        <f>B2/(1-(1/(1+B2)*(EXP(B3))))</f>
+        <v>-3.3649266577928447E-8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6">
+        <f>B5*B1</f>
+        <v>-3.3649266577928447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>